<commit_message>
Generacion biomasa paso1: lectura
</commit_message>
<xml_diff>
--- a/data/biomass/biomasa.xlsx
+++ b/data/biomass/biomasa.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateo\Documents\Trabajo de investigación\ResearchDev\data\biomass\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222438E2-A018-47E4-B103-0963E173B40D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Datos" sheetId="1" r:id="rId1"/>
+    <sheet name="Info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +25,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clasificación de residuos </t>
+  </si>
+  <si>
+    <t>RAI</t>
+  </si>
+  <si>
+    <t>RAC</t>
+  </si>
+  <si>
+    <t>Desechos aprobecables en compostaje y quema</t>
+  </si>
+  <si>
+    <t>Bagazo, cascarilla, pecuarios</t>
+  </si>
+  <si>
+    <t>RSU</t>
+  </si>
+  <si>
+    <t>Residuos municipales</t>
+  </si>
+  <si>
+    <t>Centros de abastos y plazas de mercado</t>
+  </si>
+  <si>
+    <t>PODA</t>
+  </si>
+  <si>
+    <t>Proceso de generación de biogas</t>
+  </si>
+  <si>
+    <t>fermentación metanogénica
+(proceso anaerobico)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,8 +98,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -66,6 +121,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>6785</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>120470</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{126EECE4-DFD2-9DAB-2C18-D5CE9BEC1E18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2495550" y="1685925"/>
+          <a:ext cx="7664885" cy="3254195"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>131445</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>742110</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79AB92A0-31C1-8918-406E-891A576B59D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2491740" y="4951095"/>
+          <a:ext cx="7613445" cy="4555490"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>31562</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>16075</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA01D87D-B1FC-5427-93C2-6C3A26CEB354}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2430780" y="9353550"/>
+          <a:ext cx="7754432" cy="5978725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +522,97 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182847A4-B234-4F63-A4E8-6CFF6CB60B0E}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" style="2"/>
+    <col min="2" max="2" width="22.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test: Ajustes de datos de biomasa
Cambios en recurso aprovechable
</commit_message>
<xml_diff>
--- a/data/biomass/biomasa.xlsx
+++ b/data/biomass/biomasa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateo\Documents\Trabajo de investigación\ResearchDev\data\biomass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C9FFE5-A0E2-41E3-862B-CDDCC75C751C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADB0586-606C-4708-8113-930349A72D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Recursos" sheetId="4" r:id="rId1"/>
@@ -1512,7 +1512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37D2584B-F4C1-482B-ADC0-F5EBE49A9670}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1693,8 +1693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H15:H16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1796,7 +1796,7 @@
         <v>0.4</v>
       </c>
       <c r="I3" s="27">
-        <v>4500</v>
+        <v>1500</v>
       </c>
       <c r="J3" s="28">
         <f>J2*$C$3</f>
@@ -1862,7 +1862,7 @@
         <v>0.13500000000000001</v>
       </c>
       <c r="I5" s="27">
-        <v>7300</v>
+        <v>5000</v>
       </c>
       <c r="J5" s="27">
         <f>$C$5*J2</f>
@@ -1927,7 +1927,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="I7" s="27">
-        <v>600000</v>
+        <v>100000</v>
       </c>
       <c r="J7" s="27">
         <f>$C$7*J2</f>
@@ -2074,7 +2074,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="I13" s="27">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="J13" s="28">
         <f>$C$13*J2</f>
@@ -2148,7 +2148,7 @@
         <v>41</v>
       </c>
       <c r="I16" s="28">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J16" s="28">
         <f t="shared" ref="J16:L16" si="6">$F$16*J2</f>

</xml_diff>

<commit_message>
feat: treemap para recursos de biomasa
</commit_message>
<xml_diff>
--- a/data/biomass/biomasa.xlsx
+++ b/data/biomass/biomasa.xlsx
@@ -9,8 +9,9 @@
   </bookViews>
   <sheets>
     <sheet name="Recursos" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Datos" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Info" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Recursos_old" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Datos" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Info" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t xml:space="preserve">Fuente</t>
   </si>
@@ -1077,9 +1078,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>4320</xdr:colOff>
+      <xdr:colOff>1800</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>118080</xdr:rowOff>
+      <xdr:rowOff>115560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1093,7 +1094,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2564640" y="2038320"/>
-          <a:ext cx="7908840" cy="3242160"/>
+          <a:ext cx="7906320" cy="3239640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1114,9 +1115,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>740160</xdr:colOff>
+      <xdr:colOff>737640</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1130,7 +1131,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2561040" y="5293800"/>
-          <a:ext cx="7831800" cy="4553280"/>
+          <a:ext cx="7829280" cy="4550760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1151,9 +1152,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>37080</xdr:colOff>
+      <xdr:colOff>34560</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>13680</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1167,7 +1168,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2507760" y="9696240"/>
-          <a:ext cx="7998480" cy="5976720"/>
+          <a:ext cx="7995960" cy="5974200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1188,9 +1189,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>150840</xdr:colOff>
+      <xdr:colOff>148320</xdr:colOff>
       <xdr:row>105</xdr:row>
-      <xdr:rowOff>135360</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1204,7 +1205,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2431440" y="16745040"/>
-          <a:ext cx="7372080" cy="3754800"/>
+          <a:ext cx="7369560" cy="3752280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1225,9 +1226,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>440640</xdr:colOff>
+      <xdr:colOff>438120</xdr:colOff>
       <xdr:row>139</xdr:row>
-      <xdr:rowOff>158400</xdr:rowOff>
+      <xdr:rowOff>155880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1241,7 +1242,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1037520" y="20606400"/>
-          <a:ext cx="10689120" cy="6069600"/>
+          <a:ext cx="10686600" cy="6067080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1264,6 +1265,228 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="15.66"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="15.66"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>2563</v>
+      </c>
+      <c r="C2" s="3" t="n">
+        <v>1025</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>2050</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>3075</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <v>10249</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>4600</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>1839</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>3678</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>5517</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0.135</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>18390</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>151000</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>307000</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>614000</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>921000</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>3070000</v>
+      </c>
+      <c r="H4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>124</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>247</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>370</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1235</v>
+      </c>
+      <c r="H5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>97</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>322</v>
+      </c>
+      <c r="H6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>97</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>145</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>0.075</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>28128</v>
+      </c>
+      <c r="C8" s="3" t="n">
+        <v>1406000</v>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>2813000</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>4219000</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>14064000</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="6"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1478,7 +1701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2184,7 +2407,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>

</xml_diff>

<commit_message>
feat: check availability for resources
</commit_message>
<xml_diff>
--- a/data/biomass/biomasa.xlsx
+++ b/data/biomass/biomasa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Recursos"/>
@@ -14,6 +14,9 @@
     <sheet r:id="rId5" sheetId="5" name="Historico Pecuario"/>
     <sheet r:id="rId6" sheetId="6" name="Info"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3">'Historico Cultivos'!$B$1:$B$55</definedName>
+  </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -81,7 +84,7 @@
     <t>total_farms</t>
   </si>
   <si>
-    <t>bovino</t>
+    <t>cattle</t>
   </si>
   <si>
     <t>production</t>
@@ -96,22 +99,22 @@
     <t>harvested_area</t>
   </si>
   <si>
-    <t>Caña</t>
-  </si>
-  <si>
-    <t>Arroz</t>
-  </si>
-  <si>
-    <t>Cítricos</t>
-  </si>
-  <si>
-    <t>Piña</t>
-  </si>
-  <si>
-    <t>Café</t>
-  </si>
-  <si>
-    <t>Plátano</t>
+    <t>sugar cane</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>citrus</t>
+  </si>
+  <si>
+    <t>pineapple</t>
+  </si>
+  <si>
+    <t>coffee</t>
+  </si>
+  <si>
+    <t>banana</t>
   </si>
   <si>
     <t>DATOS TOTALES 2022 - SECTOR PECUARIO ICA - INSTITUTO COLOMBIANO AGROPECUARIO</t>
@@ -248,7 +251,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -287,12 +290,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -670,7 +667,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -705,9 +702,6 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -765,9 +759,6 @@
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="3" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -786,10 +777,10 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="16" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="7" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="6" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="7" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="18" applyBorder="1" fontId="6" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="19" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
@@ -823,9 +814,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -862,31 +850,31 @@
         <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="ffffff" val="window"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0e2841"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e8e8e8"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="e97132"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196b24"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0f9ed5"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="a02b93"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4ea72e"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
         <a:srgbClr val="0000FF"/>
@@ -1148,12 +1136,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="48" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="51" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="51" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="51" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="51" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="56" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="46" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="49" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="49" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="49" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="49" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="53" width="15.719285714285713" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="10" width="15.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -1161,19 +1149,19 @@
       <c r="A1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="13">
         <v>0.1</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="13">
         <v>0.2</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="13">
         <v>0.3</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>64</v>
       </c>
       <c r="G1" s="9" t="s">
@@ -1184,22 +1172,22 @@
       <c r="A2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="54">
+      <c r="B2" s="51">
         <v>2563</v>
       </c>
-      <c r="C2" s="54">
+      <c r="C2" s="51">
         <v>1025</v>
       </c>
-      <c r="D2" s="54">
+      <c r="D2" s="51">
         <v>2050</v>
       </c>
-      <c r="E2" s="54">
+      <c r="E2" s="51">
         <v>3075</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="13">
         <v>0.4</v>
       </c>
-      <c r="G2" s="55">
+      <c r="G2" s="52">
         <v>10249</v>
       </c>
     </row>
@@ -1207,19 +1195,19 @@
       <c r="A3" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="54">
+      <c r="B3" s="51">
         <v>4600</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="51">
         <v>1839</v>
       </c>
-      <c r="D3" s="54">
+      <c r="D3" s="51">
         <v>3678</v>
       </c>
-      <c r="E3" s="54">
+      <c r="E3" s="51">
         <v>5517</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <v>0.135</v>
       </c>
       <c r="G3" s="9">
@@ -1230,19 +1218,19 @@
       <c r="A4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="54">
+      <c r="B4" s="51">
         <v>151000</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="51">
         <v>307000</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="51">
         <v>614000</v>
       </c>
-      <c r="E4" s="54">
+      <c r="E4" s="51">
         <v>921000</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>0.014</v>
       </c>
       <c r="G4" s="9">
@@ -1253,19 +1241,19 @@
       <c r="A5" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="51">
         <v>0</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="51">
         <v>124</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="51">
         <v>247</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="51">
         <v>370</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>0.4</v>
       </c>
       <c r="G5" s="9">
@@ -1276,19 +1264,19 @@
       <c r="A6" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="51">
         <v>0</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="51">
         <v>32</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="51">
         <v>64</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="51">
         <v>97</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>0.1</v>
       </c>
       <c r="G6" s="9">
@@ -1299,19 +1287,19 @@
       <c r="A7" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="54">
+      <c r="B7" s="51">
         <v>0</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="51">
         <v>48</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="51">
         <v>97</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="51">
         <v>145</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>0.075</v>
       </c>
       <c r="G7" s="9">
@@ -1322,19 +1310,19 @@
       <c r="A8" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="54">
+      <c r="B8" s="51">
         <v>28128</v>
       </c>
-      <c r="C8" s="54">
+      <c r="C8" s="51">
         <v>1406000</v>
       </c>
-      <c r="D8" s="54">
+      <c r="D8" s="51">
         <v>2813000</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="51">
         <v>4219000</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>0.25</v>
       </c>
       <c r="G8" s="9">
@@ -1357,11 +1345,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="48" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="51" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="51" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="51" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="51" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="46" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="49" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="49" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="49" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="49" width="11.576428571428572" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="10" width="15.719285714285713" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="10" width="15.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
@@ -1370,16 +1358,16 @@
       <c r="A1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="14">
+      <c r="C1" s="13">
         <v>0.1</v>
       </c>
-      <c r="D1" s="14">
+      <c r="D1" s="13">
         <v>0.2</v>
       </c>
-      <c r="E1" s="14">
+      <c r="E1" s="13">
         <v>0.3</v>
       </c>
       <c r="F1" s="7" t="s">
@@ -1393,22 +1381,22 @@
       <c r="A2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="54">
+      <c r="B2" s="51">
         <v>4000</v>
       </c>
-      <c r="C2" s="54">
+      <c r="C2" s="51">
         <v>1025</v>
       </c>
-      <c r="D2" s="54">
+      <c r="D2" s="51">
         <v>2050</v>
       </c>
-      <c r="E2" s="54">
+      <c r="E2" s="51">
         <v>3075</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="13">
         <v>0.4</v>
       </c>
-      <c r="G2" s="55">
+      <c r="G2" s="52">
         <v>10249</v>
       </c>
     </row>
@@ -1416,19 +1404,19 @@
       <c r="A3" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="54">
+      <c r="B3" s="51">
         <v>6000</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="51">
         <v>1839</v>
       </c>
-      <c r="D3" s="54">
+      <c r="D3" s="51">
         <v>3678</v>
       </c>
-      <c r="E3" s="54">
+      <c r="E3" s="51">
         <v>5517</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="13">
         <v>0.135</v>
       </c>
       <c r="G3" s="9">
@@ -1439,19 +1427,19 @@
       <c r="A4" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="54">
+      <c r="B4" s="51">
         <v>500000</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="51">
         <v>307000</v>
       </c>
-      <c r="D4" s="54">
+      <c r="D4" s="51">
         <v>614000</v>
       </c>
-      <c r="E4" s="54">
+      <c r="E4" s="51">
         <v>921000</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>0.014</v>
       </c>
       <c r="G4" s="9">
@@ -1462,19 +1450,19 @@
       <c r="A5" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="51">
         <v>0</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="51">
         <v>124</v>
       </c>
-      <c r="D5" s="54">
+      <c r="D5" s="51">
         <v>247</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="51">
         <v>370</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>0.4</v>
       </c>
       <c r="G5" s="9">
@@ -1485,19 +1473,19 @@
       <c r="A6" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="51">
         <v>0</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="51">
         <v>32</v>
       </c>
-      <c r="D6" s="54">
+      <c r="D6" s="51">
         <v>64</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="51">
         <v>97</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>0.1</v>
       </c>
       <c r="G6" s="9">
@@ -1508,19 +1496,19 @@
       <c r="A7" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="54">
+      <c r="B7" s="51">
         <v>150</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="51">
         <v>48</v>
       </c>
-      <c r="D7" s="54">
+      <c r="D7" s="51">
         <v>97</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="51">
         <v>145</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>0.075</v>
       </c>
       <c r="G7" s="9">
@@ -1531,16 +1519,16 @@
       <c r="A8" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="54">
+      <c r="B8" s="51">
         <v>15</v>
       </c>
-      <c r="C8" s="54">
+      <c r="C8" s="51">
         <v>1406000</v>
       </c>
-      <c r="D8" s="54">
+      <c r="D8" s="51">
         <v>2813000</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="51">
         <v>4219000</v>
       </c>
       <c r="F8" s="9">
@@ -1566,455 +1554,455 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="48" width="21.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="48" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="49" width="24.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="49" width="27.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="49" width="28.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="49" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="49" width="26.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="50" width="18.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="51" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="52" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="52" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="52" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="46" width="21.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="46" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="47" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="47" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="47" width="28.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="47" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="47" width="26.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="48" width="18.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="49" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="49" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="49" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="49" width="13.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="23">
         <v>0.1</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="23">
         <v>0.2</v>
       </c>
-      <c r="L2" s="24">
+      <c r="L2" s="23">
         <v>0.3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="26">
+      <c r="C3" s="25">
         <v>10249</v>
       </c>
-      <c r="D3" s="26">
+      <c r="D3" s="25">
         <v>317</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="26">
         <v>31</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="27">
         <v>16</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="26">
         <v>1</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="28">
         <v>0.4</v>
       </c>
-      <c r="I3" s="30">
+      <c r="I3" s="29">
         <v>1500</v>
       </c>
-      <c r="J3" s="31">
+      <c r="J3" s="30">
         <f>J2*$C$3</f>
       </c>
-      <c r="K3" s="31">
+      <c r="K3" s="30">
         <f>K2*$C$3</f>
       </c>
-      <c r="L3" s="31">
+      <c r="L3" s="30">
         <f>L2*$C$3</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="33" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="33" t="s">
+      <c r="G4" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="25">
         <f>3789+14601</f>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>3789</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="25">
         <v>9</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>14601</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="25">
         <v>2</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="28">
         <v>0.135</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="29">
         <v>5000</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="29">
         <f>$C$5*J2</f>
       </c>
-      <c r="K5" s="30">
+      <c r="K5" s="29">
         <f>$C$5*K2</f>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="29">
         <f>$C$5*L2</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="21" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="35">
         <v>3070000</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="27">
         <v>2700000</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="36">
         <v>20</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="25">
         <v>370000</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="36">
         <v>7</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="28">
         <v>0.014</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="29">
         <v>100000</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="29">
         <f>$C$7*J2</f>
       </c>
-      <c r="K7" s="30">
+      <c r="K7" s="29">
         <f>$C$7*K2</f>
       </c>
-      <c r="L7" s="30">
+      <c r="L7" s="29">
         <f>$C$7*L2</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="39" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40" t="s">
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <v>1235</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29">
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="28">
         <v>0.4</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="29">
         <v>0</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="30">
         <f>$C$9*J2</f>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="30">
         <f>$C$9*K2</f>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="30">
         <f>$C$9*L2</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="39" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40" t="s">
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="27">
         <v>322</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="29">
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="28">
         <v>0.1</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="29">
         <v>0</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J11" s="30">
         <f>$C$11*J2</f>
       </c>
-      <c r="K11" s="31">
+      <c r="K11" s="30">
         <f>$C$11*K2</f>
       </c>
-      <c r="L11" s="31">
+      <c r="L11" s="30">
         <f>$C$11*L2</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="39" t="s">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40" t="s">
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="27">
         <v>484</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="29">
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="28">
         <v>0.075</v>
       </c>
-      <c r="I13" s="30">
+      <c r="I13" s="29">
         <v>50</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="30">
         <f>$C$13*J2</f>
       </c>
-      <c r="K13" s="31">
+      <c r="K13" s="30">
         <f>$C$13*K2</f>
       </c>
-      <c r="L13" s="31">
+      <c r="L13" s="30">
         <f>$C$13*L2</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="45" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45" t="s">
+      <c r="E15" s="43"/>
+      <c r="F15" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="45"/>
-      <c r="H15" s="46" t="s">
+      <c r="G15" s="43"/>
+      <c r="H15" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="35">
         <v>9316</v>
       </c>
-      <c r="D16" s="37">
+      <c r="D16" s="35">
         <v>5133205.4</v>
       </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37">
+      <c r="E16" s="35"/>
+      <c r="F16" s="35">
         <f>5133205/365</f>
       </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="47" t="s">
+      <c r="G16" s="35"/>
+      <c r="H16" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="30">
         <v>10</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="30">
         <f>$F$16*J2</f>
       </c>
-      <c r="K16" s="31">
+      <c r="K16" s="30">
         <f>$F$16*K2</f>
       </c>
-      <c r="L16" s="31">
+      <c r="L16" s="30">
         <f>$F$16*L2</f>
       </c>
     </row>
@@ -2043,19 +2031,19 @@
   </sheetPr>
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="10" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="15" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="11.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="10" width="18.14785714285714" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="10" width="18.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
@@ -2065,7 +2053,7 @@
       <c r="C1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>22</v>
       </c>
       <c r="E1" s="7" t="s">
@@ -2075,7 +2063,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="9">
         <v>2022</v>
       </c>
@@ -2085,7 +2073,7 @@
       <c r="C2" s="9">
         <v>1019430</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <v>109.7</v>
       </c>
       <c r="E2" s="9">
@@ -2095,7 +2083,7 @@
         <v>9293</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="9">
         <v>2022</v>
       </c>
@@ -2105,7 +2093,7 @@
       <c r="C3" s="9">
         <v>18591</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="13">
         <v>6.02</v>
       </c>
       <c r="E3" s="9">
@@ -2115,7 +2103,7 @@
         <v>3086</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="9">
         <v>2022</v>
       </c>
@@ -2135,7 +2123,7 @@
         <v>415</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="9">
         <v>2022</v>
       </c>
@@ -2155,7 +2143,7 @@
         <v>73</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="9">
         <v>2021</v>
       </c>
@@ -2165,7 +2153,7 @@
       <c r="C6" s="9">
         <v>1019340</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="13">
         <v>109.71</v>
       </c>
       <c r="E6" s="9">
@@ -2175,7 +2163,7 @@
         <v>9292</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="9">
         <v>2021</v>
       </c>
@@ -2185,7 +2173,7 @@
       <c r="C7" s="9">
         <v>17017</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <v>5.5</v>
       </c>
       <c r="E7" s="9">
@@ -2195,7 +2183,7 @@
         <v>3093</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="9">
         <v>2021</v>
       </c>
@@ -2215,7 +2203,7 @@
         <v>427</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="9">
         <v>2021</v>
       </c>
@@ -2235,7 +2223,7 @@
         <v>73</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="9">
         <v>2020</v>
       </c>
@@ -2245,7 +2233,7 @@
       <c r="C10" s="9">
         <v>832560</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="13">
         <v>89.84</v>
       </c>
       <c r="E10" s="9">
@@ -2255,7 +2243,7 @@
         <v>9268</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="9">
         <v>2020</v>
       </c>
@@ -2265,7 +2253,7 @@
       <c r="C11" s="9">
         <v>17105</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="13">
         <v>5.5</v>
       </c>
       <c r="E11" s="9">
@@ -2275,7 +2263,7 @@
         <v>3110</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="9">
         <v>2020</v>
       </c>
@@ -2295,7 +2283,7 @@
         <v>441</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="9">
         <v>2020</v>
       </c>
@@ -2315,7 +2303,7 @@
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="9">
         <v>2019</v>
       </c>
@@ -2325,7 +2313,7 @@
       <c r="C14" s="9">
         <v>831690</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>89.83</v>
       </c>
       <c r="E14" s="9">
@@ -2335,7 +2323,7 @@
         <v>9258</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="9">
         <v>2019</v>
       </c>
@@ -2345,7 +2333,7 @@
       <c r="C15" s="9">
         <v>15242</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>5.89</v>
       </c>
       <c r="E15" s="9">
@@ -2355,7 +2343,7 @@
         <v>2586</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="9">
         <v>2019</v>
       </c>
@@ -2365,7 +2353,7 @@
       <c r="C16" s="9">
         <v>14125</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="13">
         <v>32.1</v>
       </c>
       <c r="E16" s="9">
@@ -2375,7 +2363,7 @@
         <v>440</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="9">
         <v>2019</v>
       </c>
@@ -2395,7 +2383,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="9">
         <v>2018</v>
       </c>
@@ -2405,7 +2393,7 @@
       <c r="C18" s="9">
         <v>951299</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="13">
         <v>120.69</v>
       </c>
       <c r="E18" s="9">
@@ -2415,7 +2403,7 @@
         <v>7882</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="9">
         <v>2018</v>
       </c>
@@ -2425,7 +2413,7 @@
       <c r="C19" s="9">
         <v>17696</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="13">
         <v>5.31</v>
       </c>
       <c r="E19" s="9">
@@ -2435,7 +2423,7 @@
         <v>3330</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="9">
         <v>2018</v>
       </c>
@@ -2455,7 +2443,7 @@
         <v>439</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="9">
         <v>2018</v>
       </c>
@@ -2475,7 +2463,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="9">
         <v>2018</v>
       </c>
@@ -2485,7 +2473,7 @@
       <c r="C22" s="9">
         <v>1331</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="13">
         <v>1.08</v>
       </c>
       <c r="E22" s="9">
@@ -2495,7 +2483,7 @@
         <v>1236</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="9">
         <v>2017</v>
       </c>
@@ -2505,7 +2493,7 @@
       <c r="C23" s="9">
         <v>888224</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="13">
         <v>133.29</v>
       </c>
       <c r="E23" s="9">
@@ -2515,7 +2503,7 @@
         <v>6664</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="9">
         <v>2017</v>
       </c>
@@ -2525,7 +2513,7 @@
       <c r="C24" s="9">
         <v>16688</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="13">
         <v>5.17</v>
       </c>
       <c r="E24" s="9">
@@ -2535,7 +2523,7 @@
         <v>3230</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="9">
         <v>2017</v>
       </c>
@@ -2545,7 +2533,7 @@
       <c r="C25" s="9">
         <v>10670</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="13">
         <v>24.14</v>
       </c>
       <c r="E25" s="9">
@@ -2555,7 +2543,7 @@
         <v>442</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="9">
         <v>2017</v>
       </c>
@@ -2575,7 +2563,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="9">
         <v>2017</v>
       </c>
@@ -2585,7 +2573,7 @@
       <c r="C27" s="9">
         <v>843</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="13">
         <v>0.66</v>
       </c>
       <c r="E27" s="9">
@@ -2595,7 +2583,7 @@
         <v>1281</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="9">
         <v>2016</v>
       </c>
@@ -2605,7 +2593,7 @@
       <c r="C28" s="9">
         <v>746540</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="13">
         <v>115.69</v>
       </c>
       <c r="E28" s="9">
@@ -2615,7 +2603,7 @@
         <v>6453</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="9">
         <v>2016</v>
       </c>
@@ -2625,7 +2613,7 @@
       <c r="C29" s="9">
         <v>23177</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="13">
         <v>5.86</v>
       </c>
       <c r="E29" s="9">
@@ -2635,7 +2623,7 @@
         <v>3952</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="9">
         <v>2016</v>
       </c>
@@ -2655,7 +2643,7 @@
         <v>453</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="9">
         <v>2016</v>
       </c>
@@ -2665,7 +2653,7 @@
       <c r="C31" s="9">
         <v>1366</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="13">
         <v>1.08</v>
       </c>
       <c r="E31" s="9">
@@ -2675,7 +2663,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="9">
         <v>2016</v>
       </c>
@@ -2695,7 +2683,7 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="9">
         <v>2016</v>
       </c>
@@ -2715,7 +2703,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="9">
         <v>2015</v>
       </c>
@@ -2725,7 +2713,7 @@
       <c r="C34" s="9">
         <v>829427</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="13">
         <v>102.74</v>
       </c>
       <c r="E34" s="9">
@@ -2735,7 +2723,7 @@
         <v>8073</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="9">
         <v>2015</v>
       </c>
@@ -2745,7 +2733,7 @@
       <c r="C35" s="9">
         <v>14044</v>
       </c>
-      <c r="D35" s="14">
+      <c r="D35" s="13">
         <v>4.67</v>
       </c>
       <c r="E35" s="9">
@@ -2755,7 +2743,7 @@
         <v>3005</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="9">
         <v>2015</v>
       </c>
@@ -2775,7 +2763,7 @@
         <v>453</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="9">
         <v>2015</v>
       </c>
@@ -2785,7 +2773,7 @@
       <c r="C37" s="9">
         <v>1342</v>
       </c>
-      <c r="D37" s="14">
+      <c r="D37" s="13">
         <v>1.05</v>
       </c>
       <c r="E37" s="9">
@@ -2795,7 +2783,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="9">
         <v>2015</v>
       </c>
@@ -2815,7 +2803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="9">
         <v>2015</v>
       </c>
@@ -2845,7 +2833,7 @@
       <c r="C40" s="9">
         <v>833524</v>
       </c>
-      <c r="D40" s="14">
+      <c r="D40" s="13">
         <v>108.87</v>
       </c>
       <c r="E40" s="9">
@@ -2865,7 +2853,7 @@
       <c r="C41" s="9">
         <v>23564</v>
       </c>
-      <c r="D41" s="14">
+      <c r="D41" s="13">
         <v>6.38</v>
       </c>
       <c r="E41" s="9">
@@ -2925,7 +2913,7 @@
       <c r="C44" s="9">
         <v>672</v>
       </c>
-      <c r="D44" s="14">
+      <c r="D44" s="13">
         <v>0.52</v>
       </c>
       <c r="E44" s="9">
@@ -2945,7 +2933,7 @@
       <c r="C45" s="9">
         <v>1019708</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D45" s="13">
         <v>128.95</v>
       </c>
       <c r="E45" s="9">
@@ -2965,7 +2953,7 @@
       <c r="C46" s="9">
         <v>31605</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D46" s="13">
         <v>6.25</v>
       </c>
       <c r="E46" s="9">
@@ -3005,7 +2993,7 @@
       <c r="C48" s="9">
         <v>922</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D48" s="13">
         <v>13.16</v>
       </c>
       <c r="E48" s="9">
@@ -3025,7 +3013,7 @@
       <c r="C49" s="9">
         <v>569</v>
       </c>
-      <c r="D49" s="14">
+      <c r="D49" s="13">
         <v>0.48</v>
       </c>
       <c r="E49" s="9">
@@ -3045,7 +3033,7 @@
       <c r="C50" s="9">
         <v>982780</v>
       </c>
-      <c r="D50" s="14">
+      <c r="D50" s="13">
         <v>116.04</v>
       </c>
       <c r="E50" s="9">
@@ -3065,7 +3053,7 @@
       <c r="C51" s="9">
         <v>33539</v>
       </c>
-      <c r="D51" s="14">
+      <c r="D51" s="13">
         <v>6.67</v>
       </c>
       <c r="E51" s="9">
@@ -3105,7 +3093,7 @@
       <c r="C53" s="9">
         <v>985</v>
       </c>
-      <c r="D53" s="14">
+      <c r="D53" s="13">
         <v>0.6</v>
       </c>
       <c r="E53" s="9">
@@ -3125,7 +3113,7 @@
       <c r="C54" s="9">
         <v>662</v>
       </c>
-      <c r="D54" s="14">
+      <c r="D54" s="13">
         <v>13.79</v>
       </c>
       <c r="E54" s="9">
@@ -3139,7 +3127,7 @@
       <c r="A55" s="9"/>
       <c r="B55" s="3"/>
       <c r="C55" s="9"/>
-      <c r="D55" s="13"/>
+      <c r="D55" s="12"/>
       <c r="E55" s="9"/>
       <c r="F55" s="9"/>
     </row>
@@ -3155,7 +3143,7 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3163,7 +3151,7 @@
     <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="11" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="18.14785714285714" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="10" width="18.433571428571426" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="10" width="18.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
@@ -3181,7 +3169,7 @@
       <c r="D1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="F1" s="7" t="s">

</xml_diff>

<commit_message>
feat: biogas from biomas evaluation loaded
</commit_message>
<xml_diff>
--- a/data/biomass/biomasa.xlsx
+++ b/data/biomass/biomasa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Recursos"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="75">
   <si>
     <t xml:space="preserve">Clasificación de residuos </t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>cattle</t>
+  </si>
+  <si>
+    <t>poultry</t>
+  </si>
+  <si>
+    <t>pig</t>
   </si>
   <si>
     <t>production</t>
@@ -667,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -814,6 +820,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -1141,16 +1150,16 @@
     <col min="3" max="3" style="49" width="11.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="49" width="11.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="49" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="53" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="54" width="15.719285714285713" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="10" width="15.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>41</v>
+        <v>65</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>43</v>
       </c>
       <c r="C1" s="13">
         <v>0.1</v>
@@ -1162,49 +1171,49 @@
         <v>0.3</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="51">
+        <v>68</v>
+      </c>
+      <c r="B2" s="52">
         <v>2563</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="52">
         <v>1025</v>
       </c>
-      <c r="D2" s="51">
+      <c r="D2" s="52">
         <v>2050</v>
       </c>
-      <c r="E2" s="51">
+      <c r="E2" s="52">
         <v>3075</v>
       </c>
       <c r="F2" s="13">
         <v>0.4</v>
       </c>
-      <c r="G2" s="52">
+      <c r="G2" s="53">
         <v>10249</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="51">
+        <v>69</v>
+      </c>
+      <c r="B3" s="52">
         <v>4600</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="52">
         <v>1839</v>
       </c>
-      <c r="D3" s="51">
+      <c r="D3" s="52">
         <v>3678</v>
       </c>
-      <c r="E3" s="51">
+      <c r="E3" s="52">
         <v>5517</v>
       </c>
       <c r="F3" s="13">
@@ -1216,18 +1225,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="51">
+        <v>70</v>
+      </c>
+      <c r="B4" s="52">
         <v>151000</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="52">
         <v>307000</v>
       </c>
-      <c r="D4" s="51">
+      <c r="D4" s="52">
         <v>614000</v>
       </c>
-      <c r="E4" s="51">
+      <c r="E4" s="52">
         <v>921000</v>
       </c>
       <c r="F4" s="13">
@@ -1239,18 +1248,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="51">
+        <v>71</v>
+      </c>
+      <c r="B5" s="52">
         <v>0</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="52">
         <v>124</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="52">
         <v>247</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="52">
         <v>370</v>
       </c>
       <c r="F5" s="13">
@@ -1262,18 +1271,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="51">
+        <v>72</v>
+      </c>
+      <c r="B6" s="52">
         <v>0</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="52">
         <v>32</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="52">
         <v>64</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="52">
         <v>97</v>
       </c>
       <c r="F6" s="13">
@@ -1285,18 +1294,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="51">
+        <v>73</v>
+      </c>
+      <c r="B7" s="52">
         <v>0</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="52">
         <v>48</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="52">
         <v>97</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="52">
         <v>145</v>
       </c>
       <c r="F7" s="13">
@@ -1308,18 +1317,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="51">
+        <v>74</v>
+      </c>
+      <c r="B8" s="52">
         <v>28128</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="52">
         <v>1406000</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="52">
         <v>2813000</v>
       </c>
-      <c r="E8" s="51">
+      <c r="E8" s="52">
         <v>4219000</v>
       </c>
       <c r="F8" s="13">
@@ -1356,10 +1365,10 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="50" t="s">
-        <v>41</v>
+        <v>65</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>43</v>
       </c>
       <c r="C1" s="13">
         <v>0.1</v>
@@ -1371,49 +1380,49 @@
         <v>0.3</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="51">
+        <v>68</v>
+      </c>
+      <c r="B2" s="52">
         <v>4000</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="52">
         <v>1025</v>
       </c>
-      <c r="D2" s="51">
+      <c r="D2" s="52">
         <v>2050</v>
       </c>
-      <c r="E2" s="51">
+      <c r="E2" s="52">
         <v>3075</v>
       </c>
       <c r="F2" s="13">
         <v>0.4</v>
       </c>
-      <c r="G2" s="52">
+      <c r="G2" s="53">
         <v>10249</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B3" s="51">
+        <v>69</v>
+      </c>
+      <c r="B3" s="52">
         <v>6000</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="52">
         <v>1839</v>
       </c>
-      <c r="D3" s="51">
+      <c r="D3" s="52">
         <v>3678</v>
       </c>
-      <c r="E3" s="51">
+      <c r="E3" s="52">
         <v>5517</v>
       </c>
       <c r="F3" s="13">
@@ -1425,18 +1434,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="51">
+        <v>70</v>
+      </c>
+      <c r="B4" s="52">
         <v>500000</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="52">
         <v>307000</v>
       </c>
-      <c r="D4" s="51">
+      <c r="D4" s="52">
         <v>614000</v>
       </c>
-      <c r="E4" s="51">
+      <c r="E4" s="52">
         <v>921000</v>
       </c>
       <c r="F4" s="13">
@@ -1448,18 +1457,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B5" s="51">
+        <v>71</v>
+      </c>
+      <c r="B5" s="52">
         <v>0</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="52">
         <v>124</v>
       </c>
-      <c r="D5" s="51">
+      <c r="D5" s="52">
         <v>247</v>
       </c>
-      <c r="E5" s="51">
+      <c r="E5" s="52">
         <v>370</v>
       </c>
       <c r="F5" s="13">
@@ -1471,18 +1480,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
       <c r="A6" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="51">
+        <v>72</v>
+      </c>
+      <c r="B6" s="52">
         <v>0</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="52">
         <v>32</v>
       </c>
-      <c r="D6" s="51">
+      <c r="D6" s="52">
         <v>64</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="52">
         <v>97</v>
       </c>
       <c r="F6" s="13">
@@ -1494,18 +1503,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" s="51">
+        <v>73</v>
+      </c>
+      <c r="B7" s="52">
         <v>150</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="52">
         <v>48</v>
       </c>
-      <c r="D7" s="51">
+      <c r="D7" s="52">
         <v>97</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="52">
         <v>145</v>
       </c>
       <c r="F7" s="13">
@@ -1517,18 +1526,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
       <c r="A8" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="51">
+        <v>74</v>
+      </c>
+      <c r="B8" s="52">
         <v>15</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="52">
         <v>1406000</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="52">
         <v>2813000</v>
       </c>
-      <c r="E8" s="51">
+      <c r="E8" s="52">
         <v>4219000</v>
       </c>
       <c r="F8" s="9">
@@ -1558,19 +1567,19 @@
     <col min="2" max="2" style="46" width="11.719285714285713" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="47" width="24.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="47" width="27.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="47" width="28.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="47" width="21.862142857142857" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="47" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="47" width="26.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="47" width="39.005" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="48" width="18.862142857142857" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="49" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="49" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="49" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="49" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="50" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="50" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="50" width="13.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
@@ -1580,7 +1589,7 @@
       <c r="G1" s="16"/>
       <c r="H1" s="17"/>
       <c r="I1" s="18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J1" s="18"/>
       <c r="K1" s="18"/>
@@ -1588,31 +1597,31 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G2" s="20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J2" s="23">
         <v>0.1</v>
@@ -1626,10 +1635,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="25">
         <v>10249</v>
@@ -1666,22 +1675,22 @@
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="31" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I4" s="27"/>
       <c r="J4" s="27"/>
@@ -1690,10 +1699,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C5" s="25">
         <f>3789+14601</f>
@@ -1730,22 +1739,22 @@
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="20" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H6" s="34" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
@@ -1754,10 +1763,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C7" s="35">
         <v>3070000</v>
@@ -1794,14 +1803,14 @@
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="37" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
       <c r="G8" s="37"/>
       <c r="H8" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I8" s="27"/>
       <c r="J8" s="27"/>
@@ -1810,10 +1819,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
       <c r="A9" s="24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" s="27">
         <v>1235</v>
@@ -1842,14 +1851,14 @@
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="37" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
       <c r="H10" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
@@ -1858,10 +1867,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
       <c r="A11" s="24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C11" s="27">
         <v>322</v>
@@ -1890,14 +1899,14 @@
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="37" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
@@ -1906,10 +1915,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
       <c r="A13" s="39" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C13" s="27">
         <v>484</v>
@@ -1936,7 +1945,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
       <c r="A14" s="40" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B14" s="40"/>
       <c r="C14" s="41"/>
@@ -1954,18 +1963,18 @@
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="43" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E15" s="43"/>
       <c r="F15" s="43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G15" s="43"/>
       <c r="H15" s="44" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
@@ -1974,10 +1983,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
       <c r="A16" s="24" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" s="35">
         <v>9316</v>
@@ -1991,7 +2000,7 @@
       </c>
       <c r="G16" s="35"/>
       <c r="H16" s="45" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I16" s="30">
         <v>10</v>
@@ -2031,7 +2040,7 @@
   </sheetPr>
   <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2051,16 +2060,16 @@
         <v>14</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
@@ -2068,7 +2077,7 @@
         <v>2022</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" s="9">
         <v>1019430</v>
@@ -2088,7 +2097,7 @@
         <v>2022</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C3" s="9">
         <v>18591</v>
@@ -2108,7 +2117,7 @@
         <v>2022</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" s="9">
         <v>13821</v>
@@ -2128,7 +2137,7 @@
         <v>2022</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C5" s="9">
         <v>4745</v>
@@ -2148,7 +2157,7 @@
         <v>2021</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" s="9">
         <v>1019340</v>
@@ -2168,7 +2177,7 @@
         <v>2021</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C7" s="9">
         <v>17017</v>
@@ -2188,7 +2197,7 @@
         <v>2021</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="9">
         <v>15987</v>
@@ -2208,7 +2217,7 @@
         <v>2021</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C9" s="9">
         <v>4745</v>
@@ -2228,7 +2237,7 @@
         <v>2020</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" s="9">
         <v>832560</v>
@@ -2248,7 +2257,7 @@
         <v>2020</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C11" s="9">
         <v>17105</v>
@@ -2268,7 +2277,7 @@
         <v>2020</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C12" s="9">
         <v>13230</v>
@@ -2288,7 +2297,7 @@
         <v>2020</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" s="9">
         <v>4290</v>
@@ -2308,7 +2317,7 @@
         <v>2019</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C14" s="9">
         <v>831690</v>
@@ -2328,7 +2337,7 @@
         <v>2019</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C15" s="9">
         <v>15242</v>
@@ -2348,7 +2357,7 @@
         <v>2019</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C16" s="9">
         <v>14125</v>
@@ -2368,7 +2377,7 @@
         <v>2019</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C17" s="9">
         <v>1860</v>
@@ -2388,7 +2397,7 @@
         <v>2018</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C18" s="9">
         <v>951299</v>
@@ -2408,7 +2417,7 @@
         <v>2018</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C19" s="9">
         <v>17696</v>
@@ -2428,7 +2437,7 @@
         <v>2018</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C20" s="9">
         <v>8780</v>
@@ -2448,7 +2457,7 @@
         <v>2018</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C21" s="9">
         <v>1885</v>
@@ -2468,7 +2477,7 @@
         <v>2018</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C22" s="9">
         <v>1331</v>
@@ -2488,7 +2497,7 @@
         <v>2017</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C23" s="9">
         <v>888224</v>
@@ -2508,7 +2517,7 @@
         <v>2017</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C24" s="9">
         <v>16688</v>
@@ -2528,7 +2537,7 @@
         <v>2017</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C25" s="9">
         <v>10670</v>
@@ -2548,7 +2557,7 @@
         <v>2017</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C26" s="9">
         <v>1080</v>
@@ -2568,7 +2577,7 @@
         <v>2017</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C27" s="9">
         <v>843</v>
@@ -2588,7 +2597,7 @@
         <v>2016</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C28" s="9">
         <v>746540</v>
@@ -2608,7 +2617,7 @@
         <v>2016</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C29" s="9">
         <v>23177</v>
@@ -2628,7 +2637,7 @@
         <v>2016</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C30" s="9">
         <v>9060</v>
@@ -2648,7 +2657,7 @@
         <v>2016</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C31" s="9">
         <v>1366</v>
@@ -2668,7 +2677,7 @@
         <v>2016</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C32" s="9">
         <v>1208</v>
@@ -2688,7 +2697,7 @@
         <v>2016</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C33" s="9">
         <v>1110</v>
@@ -2708,7 +2717,7 @@
         <v>2015</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C34" s="9">
         <v>829427</v>
@@ -2728,7 +2737,7 @@
         <v>2015</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C35" s="9">
         <v>14044</v>
@@ -2748,7 +2757,7 @@
         <v>2015</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C36" s="9">
         <v>9060</v>
@@ -2768,7 +2777,7 @@
         <v>2015</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C37" s="9">
         <v>1342</v>
@@ -2788,7 +2797,7 @@
         <v>2015</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C38" s="9">
         <v>930</v>
@@ -2808,7 +2817,7 @@
         <v>2015</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C39" s="9">
         <v>714</v>
@@ -2828,7 +2837,7 @@
         <v>2014</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C40" s="9">
         <v>833524</v>
@@ -2848,7 +2857,7 @@
         <v>2014</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C41" s="9">
         <v>23564</v>
@@ -2868,7 +2877,7 @@
         <v>2014</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C42" s="9">
         <v>6795</v>
@@ -2888,7 +2897,7 @@
         <v>2014</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C43" s="9">
         <v>952</v>
@@ -2908,7 +2917,7 @@
         <v>2014</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C44" s="9">
         <v>672</v>
@@ -2928,7 +2937,7 @@
         <v>2013</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C45" s="9">
         <v>1019708</v>
@@ -2948,7 +2957,7 @@
         <v>2013</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C46" s="9">
         <v>31605</v>
@@ -2968,7 +2977,7 @@
         <v>2013</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C47" s="9">
         <v>6076</v>
@@ -2988,7 +2997,7 @@
         <v>2013</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C48" s="9">
         <v>922</v>
@@ -3008,7 +3017,7 @@
         <v>2013</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C49" s="9">
         <v>569</v>
@@ -3028,7 +3037,7 @@
         <v>2012</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C50" s="9">
         <v>982780</v>
@@ -3048,7 +3057,7 @@
         <v>2012</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C51" s="9">
         <v>33539</v>
@@ -3068,7 +3077,7 @@
         <v>2012</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C52" s="9">
         <v>5964</v>
@@ -3088,7 +3097,7 @@
         <v>2012</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C53" s="9">
         <v>985</v>
@@ -3108,7 +3117,7 @@
         <v>2012</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C54" s="9">
         <v>662</v>
@@ -3143,7 +3152,7 @@
   </sheetPr>
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3203,22 +3212,50 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="9"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="A3" s="9">
+        <v>2020</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="9">
+        <v>3700000</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="9"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="A4" s="9">
+        <v>2020</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="9">
+        <v>18390</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="9"/>

</xml_diff>